<commit_message>
Se crearon las páginas de todos los paquetes | se crearon los contenidos para la sección de servicios de algunos paquetes en desarrollo. Queda pendiente ejecutar el proceso de minificación
</commit_message>
<xml_diff>
--- a/desarrollo/copa-vacations/Paquetes para la WEB Diciembre.xlsx
+++ b/desarrollo/copa-vacations/Paquetes para la WEB Diciembre.xlsx
@@ -632,7 +632,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -675,8 +675,20 @@
         <bgColor indexed="26"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -852,12 +864,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -919,62 +944,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="10" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -983,10 +960,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -999,17 +972,98 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="10" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1291,7 +1345,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1301,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:N8"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1453,1235 +1507,1235 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" s="46" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+    <row r="5" spans="1:22" s="41" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="37">
         <v>689</v>
       </c>
-      <c r="E5" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="42">
+      <c r="E5" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="37">
         <v>4</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="37">
         <v>3</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="K5" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="44" t="s">
+      <c r="L5" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="53" t="s">
+      <c r="N5" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="53" t="s">
+      <c r="O5" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="53" t="s">
+      <c r="P5" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="53" t="s">
+      <c r="Q5" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="R5" s="54" t="s">
+      <c r="R5" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="S5" s="42" t="s">
+      <c r="S5" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="23" t="s">
+      <c r="T5" s="40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="46" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:22" s="41" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="37">
         <v>959</v>
       </c>
-      <c r="E6" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="42">
+      <c r="E6" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="37">
         <v>4</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="37">
         <v>3</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="L6" s="44" t="s">
+      <c r="L6" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="M6" s="45" t="s">
+      <c r="M6" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="44" t="s">
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="T6" s="23" t="s">
+      <c r="T6" s="40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="46" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:22" s="41" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="37">
         <v>749</v>
       </c>
-      <c r="E7" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="42" t="s">
+      <c r="E7" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="37">
         <v>4</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="37">
         <v>3</v>
       </c>
-      <c r="K7" s="44" t="s">
+      <c r="K7" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="45" t="s">
+      <c r="M7" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="54"/>
-      <c r="S7" s="42" t="s">
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="T7" s="23" t="s">
+      <c r="T7" s="40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="46" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+    <row r="8" spans="1:22" s="41" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="37">
         <v>899</v>
       </c>
-      <c r="E8" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="42" t="s">
+      <c r="E8" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="37">
         <v>4</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="37">
         <v>3</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="K8" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="L8" s="42" t="s">
+      <c r="L8" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="M8" s="45" t="s">
+      <c r="M8" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="42" t="s">
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="T8" s="23" t="s">
+      <c r="T8" s="40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:22" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="37">
         <v>1749</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="27">
+      <c r="E9" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="37">
         <v>8</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="37">
         <v>7</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="K9" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="31" t="s">
+      <c r="N9" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="31" t="s">
+      <c r="O9" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="31" t="s">
+      <c r="P9" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="31" t="s">
+      <c r="Q9" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="R9" s="32" t="s">
+      <c r="R9" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="S9" s="27"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-    </row>
-    <row r="10" spans="1:22" ht="96" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="S9" s="37"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+    </row>
+    <row r="10" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="37">
         <v>789</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="27" t="s">
+      <c r="E10" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="37">
         <v>6</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="37">
         <v>5</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="28" t="s">
+      <c r="M10" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="28" t="s">
+      <c r="N10" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="O10" s="28"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="28" t="s">
+      <c r="O10" s="38"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="S10" s="27"/>
-    </row>
-    <row r="11" spans="1:22" ht="123.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="S10" s="37"/>
+    </row>
+    <row r="11" spans="1:22" s="44" customFormat="1" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="45">
         <v>1685</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="33">
+      <c r="E11" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="45">
         <v>6</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="45">
         <v>5</v>
       </c>
-      <c r="K11" s="33" t="s">
+      <c r="K11" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="L11" s="33" t="s">
+      <c r="L11" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M11" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="34" t="s">
+      <c r="N11" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="34" t="s">
+      <c r="O11" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="P11" s="34" t="s">
+      <c r="P11" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" s="34" t="s">
+      <c r="Q11" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="R11" s="35" t="s">
+      <c r="R11" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="36"/>
-    </row>
-    <row r="12" spans="1:22" s="43" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="S11" s="48"/>
+    </row>
+    <row r="12" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A12" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="50">
         <v>1155</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="49">
         <v>4</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="49">
         <v>3</v>
       </c>
-      <c r="K12" s="37" t="s">
+      <c r="K12" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="L12" s="37" t="s">
+      <c r="L12" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="37" t="s">
+      <c r="M12" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="N12" s="39" t="s">
+      <c r="N12" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="O12" s="40"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="41" t="s">
+      <c r="O12" s="52"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="S12" s="42"/>
-    </row>
-    <row r="13" spans="1:22" s="43" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="S12" s="37"/>
+    </row>
+    <row r="13" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A13" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="50">
         <v>666</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="H13" s="37" t="s">
+      <c r="H13" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="49">
         <v>4</v>
       </c>
-      <c r="J13" s="37">
+      <c r="J13" s="49">
         <v>3</v>
       </c>
-      <c r="K13" s="37" t="s">
+      <c r="K13" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="L13" s="37" t="s">
+      <c r="L13" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="M13" s="37" t="s">
+      <c r="M13" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="N13" s="37" t="s">
+      <c r="N13" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="O13" s="40"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="41" t="s">
+      <c r="O13" s="52"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="S13" s="42"/>
-    </row>
-    <row r="14" spans="1:22" s="43" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="S13" s="37"/>
+    </row>
+    <row r="14" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A14" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="50">
         <v>836</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="49">
         <v>4</v>
       </c>
-      <c r="J14" s="37">
+      <c r="J14" s="49">
         <v>3</v>
       </c>
-      <c r="K14" s="37" t="s">
+      <c r="K14" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="L14" s="37" t="s">
+      <c r="L14" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="M14" s="37" t="s">
+      <c r="M14" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="N14" s="37" t="s">
+      <c r="N14" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="O14" s="40"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="41" t="s">
+      <c r="O14" s="52"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="S14" s="51"/>
-    </row>
-    <row r="15" spans="1:22" s="43" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="S14" s="34"/>
+    </row>
+    <row r="15" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A15" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="50">
         <v>1079</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15" s="49">
         <v>4</v>
       </c>
-      <c r="J15" s="37">
+      <c r="J15" s="49">
         <v>3</v>
       </c>
-      <c r="K15" s="37" t="s">
+      <c r="K15" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="37" t="s">
+      <c r="M15" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="N15" s="37" t="s">
+      <c r="N15" s="49" t="s">
         <v>151</v>
       </c>
-      <c r="O15" s="40"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="41" t="s">
+      <c r="O15" s="52"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="S15" s="51"/>
-    </row>
-    <row r="16" spans="1:22" ht="72" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="S15" s="34"/>
+    </row>
+    <row r="16" spans="1:22" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A16" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="55">
         <v>2403</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="24">
+      <c r="E16" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="54">
         <v>8</v>
       </c>
-      <c r="J16" s="24">
+      <c r="J16" s="54">
         <v>7</v>
       </c>
-      <c r="K16" s="24" t="s">
+      <c r="K16" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="L16" s="24" t="s">
+      <c r="L16" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="24" t="s">
+      <c r="M16" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="N16" s="26" t="s">
+      <c r="N16" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="O16" s="26" t="s">
+      <c r="O16" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="P16" s="26" t="s">
+      <c r="P16" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="Q16" s="26" t="s">
+      <c r="Q16" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="R16" s="30" t="s">
+      <c r="R16" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="S16" s="29"/>
-    </row>
-    <row r="17" spans="1:19" ht="72" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="S16" s="58"/>
+    </row>
+    <row r="17" spans="1:19" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A17" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="37">
         <v>2129</v>
       </c>
-      <c r="E17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="27">
+      <c r="E17" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="37">
         <v>8</v>
       </c>
-      <c r="J17" s="27">
+      <c r="J17" s="37">
         <v>7</v>
       </c>
-      <c r="K17" s="27" t="s">
+      <c r="K17" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="L17" s="27" t="s">
+      <c r="L17" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="27" t="s">
+      <c r="M17" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="N17" s="27" t="s">
+      <c r="N17" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="O17" s="28" t="s">
+      <c r="O17" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="28" t="s">
+      <c r="P17" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="Q17" s="28" t="s">
+      <c r="Q17" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="R17" s="30" t="s">
+      <c r="R17" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="S17" s="22"/>
-    </row>
-    <row r="18" spans="1:19" ht="72" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
+      <c r="S17" s="59"/>
+    </row>
+    <row r="18" spans="1:19" s="63" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="34">
         <v>1872</v>
       </c>
-      <c r="E18" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27">
+      <c r="E18" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="64">
+        <v>8</v>
+      </c>
+      <c r="J18" s="64">
+        <v>7</v>
+      </c>
+      <c r="K18" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="L18" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="N18" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="O18" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="P18" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q18" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="R18" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="S18" s="62"/>
+    </row>
+    <row r="19" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="L19" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="S19" s="22"/>
+    </row>
+    <row r="20" spans="1:19" s="44" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="37">
+        <v>1090</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="37">
+        <v>6</v>
+      </c>
+      <c r="J20" s="37">
         <v>5</v>
       </c>
-      <c r="K18" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="N18" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="O18" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="P18" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q18" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="R18" s="30" t="s">
+      <c r="K20" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="L20" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="N20" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="O20" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="P20" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q20" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="R20" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="S18" s="22"/>
-    </row>
-    <row r="19" spans="1:19" ht="72" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="27" t="s">
+      <c r="S20" s="59"/>
+    </row>
+    <row r="21" spans="1:19" s="27" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="26">
+        <v>1150</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="26">
+        <v>6</v>
+      </c>
+      <c r="J21" s="26">
+        <v>5</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="N21" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="O21" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="P21" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q21" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="R21" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="S21" s="31"/>
+    </row>
+    <row r="22" spans="1:19" s="27" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="26">
+        <v>1440</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="26">
+        <v>6</v>
+      </c>
+      <c r="J22" s="26">
+        <v>5</v>
+      </c>
+      <c r="K22" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="L22" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="N22" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="O22" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="P22" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q22" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="R22" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="S22" s="31"/>
+    </row>
+    <row r="23" spans="1:19" s="27" customFormat="1" ht="108" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="26">
+        <v>1990</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="26">
+        <v>8</v>
+      </c>
+      <c r="J23" s="26">
+        <v>7</v>
+      </c>
+      <c r="K23" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="N23" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="O23" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="P23" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q23" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="R23" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="S23" s="31"/>
+    </row>
+    <row r="24" spans="1:19" s="27" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="27" t="s">
+      <c r="D24" s="26">
+        <v>1090</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27">
-        <v>2</v>
-      </c>
-      <c r="K19" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="L19" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="52"/>
-      <c r="P19" s="52"/>
-      <c r="Q19" s="52"/>
-      <c r="R19" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="S19" s="22"/>
-    </row>
-    <row r="20" spans="1:19" s="43" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="42">
-        <v>1090</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="42" t="s">
+      <c r="H24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="42">
-        <v>6</v>
-      </c>
-      <c r="J20" s="42">
+      <c r="I24" s="26">
         <v>5</v>
       </c>
-      <c r="K20" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="L20" s="42" t="s">
+      <c r="J24" s="26">
+        <v>4</v>
+      </c>
+      <c r="K24" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="L24" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="M20" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="N20" s="44" t="s">
+      <c r="M24" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="N24" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="O20" s="44" t="s">
+      <c r="O24" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="P20" s="44" t="s">
+      <c r="P24" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="Q20" s="44" t="s">
+      <c r="Q24" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="R20" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="S20" s="49"/>
-    </row>
-    <row r="21" spans="1:19" s="43" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="42" t="s">
+      <c r="R24" s="32"/>
+      <c r="S24" s="29"/>
+    </row>
+    <row r="25" spans="1:19" s="27" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="26">
+        <v>1097</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="26">
+        <v>5</v>
+      </c>
+      <c r="J25" s="26">
+        <v>4</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="L25" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="M25" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="N25" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+    </row>
+    <row r="26" spans="1:19" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="42">
-        <v>1150</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="42">
-        <v>6</v>
-      </c>
-      <c r="J21" s="42">
+      <c r="D26" s="26">
+        <v>1188</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="26">
         <v>5</v>
       </c>
-      <c r="K21" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="L21" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="M21" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="N21" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="O21" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="P21" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q21" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="R21" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="S21" s="49"/>
-    </row>
-    <row r="22" spans="1:19" s="43" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="42">
-        <v>1440</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="42">
-        <v>6</v>
-      </c>
-      <c r="J22" s="42">
-        <v>5</v>
-      </c>
-      <c r="K22" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="L22" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="M22" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="N22" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="O22" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="P22" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q22" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="R22" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="S22" s="49"/>
-    </row>
-    <row r="23" spans="1:19" s="43" customFormat="1" ht="108" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="D23" s="42">
-        <v>1990</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="42" t="s">
+      <c r="J26" s="26">
+        <v>4</v>
+      </c>
+      <c r="K26" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="L26" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="M26" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="N26" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+    </row>
+    <row r="27" spans="1:19" s="27" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="26">
+        <v>695</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="42">
-        <v>8</v>
-      </c>
-      <c r="J23" s="42">
-        <v>7</v>
-      </c>
-      <c r="K23" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="L23" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="M23" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="N23" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="O23" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="P23" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q23" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="R23" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="S23" s="49"/>
-    </row>
-    <row r="24" spans="1:19" s="43" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="42">
-        <v>1090</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="42">
-        <v>5</v>
-      </c>
-      <c r="J24" s="42">
+      <c r="I27" s="26">
         <v>4</v>
       </c>
-      <c r="K24" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="L24" s="42" t="s">
+      <c r="J27" s="26">
+        <v>3</v>
+      </c>
+      <c r="K27" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="L27" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="M24" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="N24" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="O24" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="P24" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q24" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="R24" s="50"/>
-      <c r="S24" s="47"/>
-    </row>
-    <row r="25" spans="1:19" s="43" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A25" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="42">
-        <v>1097</v>
-      </c>
-      <c r="E25" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="42">
-        <v>5</v>
-      </c>
-      <c r="J25" s="42">
-        <v>4</v>
-      </c>
-      <c r="K25" s="44" t="s">
-        <v>127</v>
-      </c>
-      <c r="L25" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="M25" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="N25" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="47"/>
-      <c r="S25" s="47"/>
-    </row>
-    <row r="26" spans="1:19" s="43" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="42">
-        <v>1188</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="42">
-        <v>5</v>
-      </c>
-      <c r="J26" s="42">
-        <v>4</v>
-      </c>
-      <c r="K26" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="L26" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="M26" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="N26" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="47"/>
-      <c r="S26" s="47"/>
-    </row>
-    <row r="27" spans="1:19" s="43" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="42">
-        <v>695</v>
-      </c>
-      <c r="E27" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="42">
-        <v>4</v>
-      </c>
-      <c r="J27" s="42">
-        <v>3</v>
-      </c>
-      <c r="K27" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="L27" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="M27" s="44" t="s">
+      <c r="M27" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="N27" s="42" t="s">
+      <c r="N27" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="47"/>
-      <c r="S27" s="47"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
     </row>
     <row r="28" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
@@ -3390,7 +3444,14 @@
       <c r="Q61" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
     <mergeCell ref="P18:P19"/>
     <mergeCell ref="Q18:Q19"/>
     <mergeCell ref="S14:S15"/>
@@ -3399,11 +3460,6 @@
     <mergeCell ref="P5:P8"/>
     <mergeCell ref="Q5:Q8"/>
     <mergeCell ref="R5:R8"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="R5" r:id="rId1" display="www.copavacations.com.co"/>

</xml_diff>

<commit_message>
avanzando con los servicios...
</commit_message>
<xml_diff>
--- a/desarrollo/copa-vacations/Paquetes para la WEB Diciembre.xlsx
+++ b/desarrollo/copa-vacations/Paquetes para la WEB Diciembre.xlsx
@@ -632,7 +632,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -667,12 +667,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor indexed="26"/>
       </patternFill>
     </fill>
     <fill>
@@ -882,7 +876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -941,18 +935,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -963,17 +945,73 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="10" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -984,85 +1022,16 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="10" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1345,7 +1314,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1355,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1507,901 +1476,901 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" s="41" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+    <row r="5" spans="1:22" s="31" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="27">
         <v>689</v>
       </c>
-      <c r="E5" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="37">
+      <c r="E5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="27">
         <v>4</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="27">
         <v>3</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="39" t="s">
+      <c r="M5" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="35" t="s">
+      <c r="O5" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="35" t="s">
+      <c r="Q5" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="R5" s="36" t="s">
+      <c r="R5" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="S5" s="37" t="s">
+      <c r="S5" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="40" t="s">
+      <c r="T5" s="30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="41" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:22" s="31" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="27">
         <v>959</v>
       </c>
-      <c r="E6" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="37">
+      <c r="E6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="27">
         <v>4</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="27">
         <v>3</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="38" t="s">
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="52"/>
+      <c r="S6" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="T6" s="40" t="s">
+      <c r="T6" s="30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="41" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:22" s="31" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="27">
         <v>749</v>
       </c>
-      <c r="E7" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="37" t="s">
+      <c r="E7" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="27">
         <v>4</v>
       </c>
-      <c r="J7" s="37">
+      <c r="J7" s="27">
         <v>3</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="37" t="s">
+      <c r="L7" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="37" t="s">
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="T7" s="40" t="s">
+      <c r="T7" s="30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="41" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:22" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="27">
         <v>899</v>
       </c>
-      <c r="E8" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="37" t="s">
+      <c r="E8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="27">
         <v>4</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="27">
         <v>3</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L8" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="M8" s="39" t="s">
+      <c r="M8" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="36"/>
-      <c r="S8" s="37" t="s">
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="T8" s="40" t="s">
+      <c r="T8" s="30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+    <row r="9" spans="1:22" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="27">
         <v>1749</v>
       </c>
-      <c r="E9" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="37">
+      <c r="E9" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="27">
         <v>8</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="27">
         <v>7</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="N9" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="42" t="s">
+      <c r="O9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="42" t="s">
+      <c r="P9" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="42" t="s">
+      <c r="Q9" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="R9" s="43" t="s">
+      <c r="R9" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="S9" s="37"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-    </row>
-    <row r="10" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="S9" s="27"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+    </row>
+    <row r="10" spans="1:22" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="27">
         <v>789</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="37" t="s">
+      <c r="E10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="27">
         <v>6</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="27">
         <v>5</v>
       </c>
-      <c r="K10" s="38" t="s">
+      <c r="K10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="38" t="s">
+      <c r="M10" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="38" t="s">
+      <c r="N10" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="O10" s="38"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="38" t="s">
+      <c r="O10" s="28"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="S10" s="37"/>
-    </row>
-    <row r="11" spans="1:22" s="44" customFormat="1" ht="123.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="S10" s="27"/>
+    </row>
+    <row r="11" spans="1:22" s="34" customFormat="1" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="35">
         <v>1685</v>
       </c>
-      <c r="E11" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="45">
+      <c r="E11" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="35">
         <v>6</v>
       </c>
-      <c r="J11" s="45">
+      <c r="J11" s="35">
         <v>5</v>
       </c>
-      <c r="K11" s="45" t="s">
+      <c r="K11" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="L11" s="45" t="s">
+      <c r="L11" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="M11" s="45" t="s">
+      <c r="M11" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="46" t="s">
+      <c r="N11" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="46" t="s">
+      <c r="O11" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="P11" s="46" t="s">
+      <c r="P11" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" s="46" t="s">
+      <c r="Q11" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="R11" s="47" t="s">
+      <c r="R11" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="48"/>
-    </row>
-    <row r="12" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="S11" s="38"/>
+    </row>
+    <row r="12" spans="1:22" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="40">
         <v>1155</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="H12" s="49" t="s">
+      <c r="H12" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="I12" s="49">
+      <c r="I12" s="39">
         <v>4</v>
       </c>
-      <c r="J12" s="49">
+      <c r="J12" s="39">
         <v>3</v>
       </c>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="L12" s="49" t="s">
+      <c r="L12" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="49" t="s">
+      <c r="M12" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="N12" s="51" t="s">
+      <c r="N12" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="O12" s="52"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="53" t="s">
+      <c r="O12" s="42"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="S12" s="37"/>
-    </row>
-    <row r="13" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="S12" s="27"/>
+    </row>
+    <row r="13" spans="1:22" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="40">
         <v>666</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="H13" s="49" t="s">
+      <c r="H13" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="I13" s="49">
+      <c r="I13" s="39">
         <v>4</v>
       </c>
-      <c r="J13" s="49">
+      <c r="J13" s="39">
         <v>3</v>
       </c>
-      <c r="K13" s="49" t="s">
+      <c r="K13" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="L13" s="49" t="s">
+      <c r="L13" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="M13" s="49" t="s">
+      <c r="M13" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="N13" s="49" t="s">
+      <c r="N13" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="O13" s="52"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="53" t="s">
+      <c r="O13" s="42"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="S13" s="37"/>
-    </row>
-    <row r="14" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
+      <c r="S13" s="27"/>
+    </row>
+    <row r="14" spans="1:22" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D14" s="40">
         <v>836</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="49" t="s">
+      <c r="H14" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="I14" s="49">
+      <c r="I14" s="39">
         <v>4</v>
       </c>
-      <c r="J14" s="49">
+      <c r="J14" s="39">
         <v>3</v>
       </c>
-      <c r="K14" s="49" t="s">
+      <c r="K14" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="L14" s="49" t="s">
+      <c r="L14" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="M14" s="49" t="s">
+      <c r="M14" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="N14" s="49" t="s">
+      <c r="N14" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="O14" s="52"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="53" t="s">
+      <c r="O14" s="42"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="S14" s="34"/>
-    </row>
-    <row r="15" spans="1:22" s="44" customFormat="1" ht="96" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="S14" s="50"/>
+    </row>
+    <row r="15" spans="1:22" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="40">
         <v>1079</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="H15" s="49" t="s">
+      <c r="H15" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="I15" s="49">
+      <c r="I15" s="39">
         <v>4</v>
       </c>
-      <c r="J15" s="49">
+      <c r="J15" s="39">
         <v>3</v>
       </c>
-      <c r="K15" s="49" t="s">
+      <c r="K15" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="L15" s="49" t="s">
+      <c r="L15" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="49" t="s">
+      <c r="M15" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="N15" s="49" t="s">
+      <c r="N15" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="O15" s="52"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="53" t="s">
+      <c r="O15" s="42"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="S15" s="34"/>
-    </row>
-    <row r="16" spans="1:22" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
+      <c r="S15" s="50"/>
+    </row>
+    <row r="16" spans="1:22" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A16" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="45">
         <v>2403</v>
       </c>
-      <c r="E16" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="54">
+      <c r="E16" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="44">
         <v>8</v>
       </c>
-      <c r="J16" s="54">
+      <c r="J16" s="44">
         <v>7</v>
       </c>
-      <c r="K16" s="54" t="s">
+      <c r="K16" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="L16" s="54" t="s">
+      <c r="L16" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="54" t="s">
+      <c r="M16" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="N16" s="56" t="s">
+      <c r="N16" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="O16" s="56" t="s">
+      <c r="O16" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="P16" s="56" t="s">
+      <c r="P16" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="Q16" s="56" t="s">
+      <c r="Q16" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="R16" s="57" t="s">
+      <c r="R16" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="S16" s="58"/>
-    </row>
-    <row r="17" spans="1:19" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A17" s="54" t="s">
+      <c r="S16" s="48"/>
+    </row>
+    <row r="17" spans="1:19" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="37">
+      <c r="D17" s="27">
         <v>2129</v>
       </c>
-      <c r="E17" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="37">
+      <c r="E17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="27">
         <v>8</v>
       </c>
-      <c r="J17" s="37">
+      <c r="J17" s="27">
         <v>7</v>
       </c>
-      <c r="K17" s="37" t="s">
+      <c r="K17" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="L17" s="37" t="s">
+      <c r="L17" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="37" t="s">
+      <c r="M17" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="N17" s="37" t="s">
+      <c r="N17" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="O17" s="38" t="s">
+      <c r="O17" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="38" t="s">
+      <c r="P17" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="Q17" s="38" t="s">
+      <c r="Q17" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="R17" s="57" t="s">
+      <c r="R17" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="S17" s="59"/>
-    </row>
-    <row r="18" spans="1:19" s="63" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="S17" s="49"/>
+    </row>
+    <row r="18" spans="1:19" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A18" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="53">
         <v>1872</v>
       </c>
-      <c r="E18" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="64">
+      <c r="E18" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="54">
         <v>8</v>
       </c>
-      <c r="J18" s="64">
+      <c r="J18" s="54">
         <v>7</v>
       </c>
-      <c r="K18" s="60" t="s">
+      <c r="K18" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="L18" s="60" t="s">
+      <c r="L18" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="M18" s="34" t="s">
+      <c r="M18" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="O18" s="33" t="s">
+      <c r="O18" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="P18" s="33" t="s">
+      <c r="P18" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="Q18" s="33" t="s">
+      <c r="Q18" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="R18" s="61" t="s">
+      <c r="R18" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="S18" s="62"/>
-    </row>
-    <row r="19" spans="1:19" ht="72" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="23" t="s">
+      <c r="S18" s="49"/>
+    </row>
+    <row r="19" spans="1:19" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A19" s="53"/>
+      <c r="B19" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="23" t="s">
+      <c r="D19" s="53"/>
+      <c r="E19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="24" t="s">
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="25" t="s">
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="S19" s="22"/>
-    </row>
-    <row r="20" spans="1:19" s="44" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="S19" s="49"/>
+    </row>
+    <row r="20" spans="1:19" s="34" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D20" s="27">
         <v>1090</v>
       </c>
-      <c r="E20" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="37" t="s">
+      <c r="E20" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="37">
+      <c r="I20" s="27">
         <v>6</v>
       </c>
-      <c r="J20" s="37">
+      <c r="J20" s="27">
         <v>5</v>
       </c>
-      <c r="K20" s="37" t="s">
+      <c r="K20" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="37" t="s">
+      <c r="L20" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="M20" s="37" t="s">
+      <c r="M20" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="N20" s="38" t="s">
+      <c r="N20" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="O20" s="38" t="s">
+      <c r="O20" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="P20" s="38" t="s">
+      <c r="P20" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="Q20" s="38" t="s">
+      <c r="Q20" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="R20" s="57" t="s">
+      <c r="R20" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="S20" s="59"/>
-    </row>
-    <row r="21" spans="1:19" s="27" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="S20" s="49"/>
+    </row>
+    <row r="21" spans="1:19" s="34" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="27">
         <v>1150</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="26">
+      <c r="E21" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="27">
         <v>6</v>
       </c>
-      <c r="J21" s="26">
+      <c r="J21" s="27">
         <v>5</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="K21" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="L21" s="26" t="s">
+      <c r="L21" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M21" s="26" t="s">
+      <c r="M21" s="27" t="s">
         <v>102</v>
       </c>
       <c r="N21" s="28" t="s">
@@ -2416,49 +2385,49 @@
       <c r="Q21" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="R21" s="30" t="s">
+      <c r="R21" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="S21" s="31"/>
-    </row>
-    <row r="22" spans="1:19" s="27" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="S21" s="49"/>
+    </row>
+    <row r="22" spans="1:19" s="34" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="27">
         <v>1440</v>
       </c>
-      <c r="E22" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="26">
+      <c r="E22" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="27">
         <v>6</v>
       </c>
-      <c r="J22" s="26">
+      <c r="J22" s="27">
         <v>5</v>
       </c>
-      <c r="K22" s="26" t="s">
+      <c r="K22" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="L22" s="26" t="s">
+      <c r="L22" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M22" s="26" t="s">
+      <c r="M22" s="27" t="s">
         <v>102</v>
       </c>
       <c r="N22" s="28" t="s">
@@ -2473,49 +2442,49 @@
       <c r="Q22" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="R22" s="30" t="s">
+      <c r="R22" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="S22" s="31"/>
-    </row>
-    <row r="23" spans="1:19" s="27" customFormat="1" ht="108" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="S22" s="49"/>
+    </row>
+    <row r="23" spans="1:19" s="34" customFormat="1" ht="108" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="27">
         <v>1990</v>
       </c>
-      <c r="E23" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="26" t="s">
+      <c r="E23" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="27">
         <v>8</v>
       </c>
-      <c r="J23" s="26">
+      <c r="J23" s="27">
         <v>7</v>
       </c>
-      <c r="K23" s="26" t="s">
+      <c r="K23" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="L23" s="26" t="s">
+      <c r="L23" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="M23" s="26" t="s">
+      <c r="M23" s="27" t="s">
         <v>102</v>
       </c>
       <c r="N23" s="28" t="s">
@@ -2530,212 +2499,212 @@
       <c r="Q23" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="R23" s="30" t="s">
+      <c r="R23" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="S23" s="31"/>
-    </row>
-    <row r="24" spans="1:19" s="27" customFormat="1" ht="144" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="S23" s="49"/>
+    </row>
+    <row r="24" spans="1:19" s="23" customFormat="1" ht="144" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="22">
         <v>1090</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="26" t="s">
+      <c r="E24" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H24" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="22">
         <v>5</v>
       </c>
-      <c r="J24" s="26">
+      <c r="J24" s="22">
         <v>4</v>
       </c>
-      <c r="K24" s="26" t="s">
+      <c r="K24" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="L24" s="26" t="s">
+      <c r="L24" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="M24" s="28" t="s">
+      <c r="M24" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="N24" s="28" t="s">
+      <c r="N24" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="O24" s="28" t="s">
+      <c r="O24" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="P24" s="28" t="s">
+      <c r="P24" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="Q24" s="28" t="s">
+      <c r="Q24" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="R24" s="32"/>
-      <c r="S24" s="29"/>
-    </row>
-    <row r="25" spans="1:19" s="27" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="R24" s="26"/>
+      <c r="S24" s="25"/>
+    </row>
+    <row r="25" spans="1:19" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="22">
         <v>1097</v>
       </c>
-      <c r="E25" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="26">
+      <c r="E25" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="22">
         <v>5</v>
       </c>
-      <c r="J25" s="26">
+      <c r="J25" s="22">
         <v>4</v>
       </c>
-      <c r="K25" s="28" t="s">
+      <c r="K25" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="L25" s="26" t="s">
+      <c r="L25" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="M25" s="28" t="s">
+      <c r="M25" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="N25" s="26" t="s">
+      <c r="N25" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="29"/>
-      <c r="S25" s="29"/>
-    </row>
-    <row r="26" spans="1:19" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+    </row>
+    <row r="26" spans="1:19" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="22">
         <v>1188</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="26">
+      <c r="E26" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="22">
         <v>5</v>
       </c>
-      <c r="J26" s="26">
+      <c r="J26" s="22">
         <v>4</v>
       </c>
-      <c r="K26" s="26" t="s">
+      <c r="K26" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="L26" s="26" t="s">
+      <c r="L26" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="M26" s="26" t="s">
+      <c r="M26" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="N26" s="26" t="s">
+      <c r="N26" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="29"/>
-      <c r="S26" s="29"/>
-    </row>
-    <row r="27" spans="1:19" s="27" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+    </row>
+    <row r="27" spans="1:19" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="22">
         <v>695</v>
       </c>
-      <c r="E27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="26" t="s">
+      <c r="E27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="26">
+      <c r="I27" s="22">
         <v>4</v>
       </c>
-      <c r="J27" s="26">
+      <c r="J27" s="22">
         <v>3</v>
       </c>
-      <c r="K27" s="26" t="s">
+      <c r="K27" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="L27" s="26" t="s">
+      <c r="L27" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="M27" s="28" t="s">
+      <c r="M27" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="N27" s="26" t="s">
+      <c r="N27" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="29"/>
-      <c r="S27" s="29"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
     </row>
     <row r="28" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
@@ -3445,13 +3414,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
     <mergeCell ref="P18:P19"/>
     <mergeCell ref="Q18:Q19"/>
     <mergeCell ref="S14:S15"/>
@@ -3460,6 +3422,13 @@
     <mergeCell ref="P5:P8"/>
     <mergeCell ref="Q5:Q8"/>
     <mergeCell ref="R5:R8"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="R5" r:id="rId1" display="www.copavacations.com.co"/>

</xml_diff>

<commit_message>
finalización de paquetes diciembre
</commit_message>
<xml_diff>
--- a/desarrollo/copa-vacations/Paquetes para la WEB Diciembre.xlsx
+++ b/desarrollo/copa-vacations/Paquetes para la WEB Diciembre.xlsx
@@ -1013,6 +1013,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,9 +1030,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1314,7 +1314,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1516,19 +1516,19 @@
       <c r="M5" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="51" t="s">
+      <c r="N5" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="51" t="s">
+      <c r="O5" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="51" t="s">
+      <c r="P5" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="51" t="s">
+      <c r="Q5" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="R5" s="52" t="s">
+      <c r="R5" s="53" t="s">
         <v>62</v>
       </c>
       <c r="S5" s="27" t="s">
@@ -1578,11 +1578,11 @@
       <c r="M6" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="53"/>
       <c r="S6" s="28" t="s">
         <v>68</v>
       </c>
@@ -1630,11 +1630,11 @@
       <c r="M7" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="53"/>
       <c r="S7" s="27" t="s">
         <v>73</v>
       </c>
@@ -1682,11 +1682,11 @@
       <c r="M8" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="51"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="53"/>
       <c r="S8" s="27" t="s">
         <v>77</v>
       </c>
@@ -2013,7 +2013,7 @@
       <c r="R14" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="S14" s="50"/>
+      <c r="S14" s="51"/>
     </row>
     <row r="15" spans="1:22" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
@@ -2064,7 +2064,7 @@
       <c r="R15" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="S15" s="50"/>
+      <c r="S15" s="51"/>
     </row>
     <row r="16" spans="1:22" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
@@ -2181,7 +2181,7 @@
       <c r="S17" s="49"/>
     </row>
     <row r="18" spans="1:19" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="54" t="s">
         <v>96</v>
       </c>
       <c r="B18" s="27" t="s">
@@ -2190,7 +2190,7 @@
       <c r="C18" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="53">
+      <c r="D18" s="54">
         <v>1872</v>
       </c>
       <c r="E18" s="27" t="s">
@@ -2205,10 +2205,10 @@
       <c r="H18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="54">
+      <c r="I18" s="55">
         <v>8</v>
       </c>
-      <c r="J18" s="54">
+      <c r="J18" s="55">
         <v>7</v>
       </c>
       <c r="K18" s="27" t="s">
@@ -2217,19 +2217,19 @@
       <c r="L18" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="M18" s="53" t="s">
+      <c r="M18" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="N18" s="53" t="s">
+      <c r="N18" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="O18" s="55" t="s">
+      <c r="O18" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="P18" s="55" t="s">
+      <c r="P18" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="Q18" s="55" t="s">
+      <c r="Q18" s="50" t="s">
         <v>93</v>
       </c>
       <c r="R18" s="47" t="s">
@@ -2238,14 +2238,14 @@
       <c r="S18" s="49"/>
     </row>
     <row r="19" spans="1:19" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="27" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="53"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="27" t="s">
         <v>14</v>
       </c>
@@ -2266,11 +2266,11 @@
       <c r="L19" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
       <c r="R19" s="47" t="s">
         <v>107</v>
       </c>
@@ -3414,6 +3414,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
     <mergeCell ref="P18:P19"/>
     <mergeCell ref="Q18:Q19"/>
     <mergeCell ref="S14:S15"/>
@@ -3422,13 +3429,6 @@
     <mergeCell ref="P5:P8"/>
     <mergeCell ref="Q5:Q8"/>
     <mergeCell ref="R5:R8"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="R5" r:id="rId1" display="www.copavacations.com.co"/>

</xml_diff>